<commit_message>
Rename driver to driver controls
</commit_message>
<xml_diff>
--- a/docs/_static/Battery Management System CAN Communication Protocol.xlsx
+++ b/docs/_static/Battery Management System CAN Communication Protocol.xlsx
@@ -218,7 +218,7 @@
     <t>Statuses</t>
   </si>
   <si>
-    <t>[0: relay status][1-63: reserved]</t>
+    <t>[0: relay status][1: electric safe discharge status][2: discharge status][3-63: reserved]</t>
   </si>
   <si>
     <t>Overvoltage/temperature/current flags</t>
@@ -248,7 +248,7 @@
     <t>Discharge</t>
   </si>
   <si>
-    <t>Unflag</t>
+    <t>Clear</t>
   </si>
   <si>
     <t>4-31</t>
@@ -1099,7 +1099,7 @@
         <v>74</v>
       </c>
       <c r="C3" s="7">
-        <v>48.0</v>
+        <v>32.0</v>
       </c>
       <c r="D3" s="7">
         <v>0.0</v>

</xml_diff>

<commit_message>
Update CAN protocols for BMS
</commit_message>
<xml_diff>
--- a/docs/_static/Battery Management System CAN Communication Protocol.xlsx
+++ b/docs/_static/Battery Management System CAN Communication Protocol.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="80">
   <si>
     <t>Type</t>
   </si>
@@ -251,7 +251,7 @@
     <t>Clear</t>
   </si>
   <si>
-    <t>4-31</t>
+    <t>5-31</t>
   </si>
 </sst>
 </file>
@@ -1014,16 +1014,15 @@
       <c r="E34" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="F34" s="7" t="s">
-        <v>73</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
     <mergeCell ref="B3:B29"/>
     <mergeCell ref="B30:B33"/>
     <mergeCell ref="E31:F31"/>
     <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:D1"/>
@@ -1031,7 +1030,6 @@
     <mergeCell ref="A3:A20"/>
     <mergeCell ref="C3:C34"/>
     <mergeCell ref="A21:A29"/>
-    <mergeCell ref="E33:F33"/>
   </mergeCells>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -1107,9 +1105,6 @@
       <c r="E3" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
@@ -1118,12 +1113,6 @@
       <c r="D4" s="7">
         <v>1.0</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
@@ -1132,12 +1121,6 @@
       <c r="D5" s="7">
         <v>2.0</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
@@ -1146,38 +1129,41 @@
       <c r="D6" s="7">
         <v>3.0</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="D7" s="7">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="B8" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>73</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="E32:F32"/>
+  <mergeCells count="10">
     <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="C3:C7"/>
-    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="C3:C8"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="E3:F8"/>
   </mergeCells>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>